<commit_message>
check box to send the Check list to ARIA
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/check_protocol/v19/ORL.xlsx
+++ b/Plancheck/plancheck_data/check_protocol/v19/ORL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="194">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -1594,8 +1594,8 @@
   </sheetPr>
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1724,9 +1724,7 @@
       <c r="A8" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>35</v>
-      </c>
+      <c r="B8" s="18"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -2896,7 +2894,7 @@
   </sheetPr>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>